<commit_message>
Add "formula" and "style" tags.  New attributes for "agg" tag and "span" tag.  Expose POI "cell".  Create and use JettFuncs.  Create readme.txt.  Create model package with enums, moving a few other classes there too.  Allow static methods to be resolved in JEXL.  Several bug fixes.
</commit_message>
<xml_diff>
--- a/jett-core/templates/AggTagTemplate.xlsx
+++ b/jett-core/templates/AggTagTemplate.xlsx
@@ -8,13 +8,18 @@
   </bookViews>
   <sheets>
     <sheet name="Agg" sheetId="1" r:id="rId1"/>
+    <sheet name="Msd" sheetId="2" r:id="rId2"/>
+    <sheet name="Rollup" sheetId="3" r:id="rId3"/>
+    <sheet name="Rollups" sheetId="4" r:id="rId4"/>
+    <sheet name="Cube" sheetId="5" r:id="rId5"/>
+    <sheet name="GroupingSets" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="23">
   <si>
     <t>${value.getAggregateValue(aggs[0])}</t>
   </si>
@@ -71,11 +76,50 @@
   <si>
     <t>${value.getAggregateValue(aggs[2])}&lt;/jt:forEach&gt;&lt;/jt:agg&gt;</t>
   </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Total Salary</t>
+  </si>
+  <si>
+    <t>${value.getAggregateValue(0)}&lt;/jt:forEach&gt;&lt;/jt:agg&gt;</t>
+  </si>
+  <si>
+    <t>&lt;jt:agg items="${employees}" aggs="Sum(salary)" valuesVar="values" groupBy="isManager()" useMsd="true"&gt;&lt;jt:forEach items="${values}" var="value"&gt;${value.getPropertyValue(0)}</t>
+  </si>
+  <si>
+    <t>Is A Manager</t>
+  </si>
+  <si>
+    <t>${value.isGrouping(1) ? 'All Values' : value.getPropertyValue(1)}</t>
+  </si>
+  <si>
+    <t>&lt;jt:agg items="${employees}" aggs="Sum(salary)" valuesVar="values" groupBy="isManager();title" rollup="${[0, 1]}"&gt;&lt;jt:forEach items="${values}" var="value" orderBy="getPropertyValue(0);getPropertyValue(1)"&gt;${value.isGrouping(0) ? 'All Values' : value.getPropertyValue(0)}</t>
+  </si>
+  <si>
+    <t>Catch Phrase</t>
+  </si>
+  <si>
+    <t>${value.isGrouping(2) ? 'All Values' : value.getPropertyValue(2)}</t>
+  </si>
+  <si>
+    <t>&lt;jt:agg items="${employees}" aggs="Sum(salary)" valuesVar="values" groupBy="isManager();title;catchPhrase" rollups="${[[1], [2]]}"&gt;&lt;jt:forEach items="${values}" var="value" orderBy="getPropertyValue(0);getPropertyValue(1);getPropertyValue(2)"&gt;${value.isGrouping(0) ? 'All Values' : value.getPropertyValue(0)}</t>
+  </si>
+  <si>
+    <t>&lt;jt:agg items="${employees}" aggs="Sum(salary)" valuesVar="values" groupBy="isManager();title;catchPhrase" cube="${[0, 1, 2]}"&gt;&lt;jt:forEach items="${values}" var="value" orderBy="getPropertyValue(0);getPropertyValue(1);getPropertyValue(2)"&gt;${value.isGrouping(0) ? 'All Values' : value.getPropertyValue(0)}</t>
+  </si>
+  <si>
+    <t>&lt;jt:agg items="${employees}" aggs="Sum(salary)" valuesVar="values" groupBy="isManager();title;catchPhrase" groupingSets="${[[0], [1, 2]]}"&gt;&lt;jt:forEach items="${values}" var="value" orderBy="getPropertyValue(0);getPropertyValue(1);getPropertyValue(2)"&gt;${value.isGrouping(0) ? 'All Values' : value.getPropertyValue(0)}</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -108,12 +152,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF99CCFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -143,12 +193,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -467,12 +519,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
     </row>
     <row r="2" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -503,12 +555,12 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
     </row>
     <row r="5" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -546,4 +598,215 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="26.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="26.42578125" customWidth="1"/>
+    <col min="3" max="3" width="31" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="26.42578125" customWidth="1"/>
+    <col min="3" max="3" width="31" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="26.42578125" customWidth="1"/>
+    <col min="3" max="3" width="31" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Bump to 0.6.0-SNAPSHOT.  Use new FormattingRun in RichTextStringUtil.  Support BigDecimals and BigIntegers as values.  Fix bug with unclosed double-quote in cell value.  Created new JDBCExecutor functionality, to execute SQL queries from the template.  Use File not FileInputStream if possible; transform methods to transform a given Workbook.
</commit_message>
<xml_diff>
--- a/jett-core/templates/AggTagTemplate.xlsx
+++ b/jett-core/templates/AggTagTemplate.xlsx
@@ -86,31 +86,31 @@
     <t>${value.getAggregateValue(0)}&lt;/jt:forEach&gt;&lt;/jt:agg&gt;</t>
   </si>
   <si>
-    <t>&lt;jt:agg items="${employees}" aggs="Sum(salary)" valuesVar="values" groupBy="isManager()" useMsd="true"&gt;&lt;jt:forEach items="${values}" var="value"&gt;${value.getPropertyValue(0)}</t>
-  </si>
-  <si>
     <t>Is A Manager</t>
   </si>
   <si>
     <t>${value.isGrouping(1) ? 'All Values' : value.getPropertyValue(1)}</t>
   </si>
   <si>
-    <t>&lt;jt:agg items="${employees}" aggs="Sum(salary)" valuesVar="values" groupBy="isManager();title" rollup="${[0, 1]}"&gt;&lt;jt:forEach items="${values}" var="value" orderBy="getPropertyValue(0);getPropertyValue(1)"&gt;${value.isGrouping(0) ? 'All Values' : value.getPropertyValue(0)}</t>
-  </si>
-  <si>
     <t>Catch Phrase</t>
   </si>
   <si>
     <t>${value.isGrouping(2) ? 'All Values' : value.getPropertyValue(2)}</t>
   </si>
   <si>
-    <t>&lt;jt:agg items="${employees}" aggs="Sum(salary)" valuesVar="values" groupBy="isManager();title;catchPhrase" rollups="${[[1], [2]]}"&gt;&lt;jt:forEach items="${values}" var="value" orderBy="getPropertyValue(0);getPropertyValue(1);getPropertyValue(2)"&gt;${value.isGrouping(0) ? 'All Values' : value.getPropertyValue(0)}</t>
-  </si>
-  <si>
-    <t>&lt;jt:agg items="${employees}" aggs="Sum(salary)" valuesVar="values" groupBy="isManager();title;catchPhrase" cube="${[0, 1, 2]}"&gt;&lt;jt:forEach items="${values}" var="value" orderBy="getPropertyValue(0);getPropertyValue(1);getPropertyValue(2)"&gt;${value.isGrouping(0) ? 'All Values' : value.getPropertyValue(0)}</t>
-  </si>
-  <si>
-    <t>&lt;jt:agg items="${employees}" aggs="Sum(salary)" valuesVar="values" groupBy="isManager();title;catchPhrase" groupingSets="${[[0], [1, 2]]}"&gt;&lt;jt:forEach items="${values}" var="value" orderBy="getPropertyValue(0);getPropertyValue(1);getPropertyValue(2)"&gt;${value.isGrouping(0) ? 'All Values' : value.getPropertyValue(0)}</t>
+    <t>&lt;jt:agg items="${employees}" aggs="Sum(salary)" valuesVar="values" groupBy="isAManager();title;catchPhrase" groupingSets="${[[0], [1, 2]]}"&gt;&lt;jt:forEach items="${values}" var="value" orderBy="getPropertyValue(0);getPropertyValue(1);getPropertyValue(2)"&gt;${value.isGrouping(0) ? 'All Values' : value.getPropertyValue(0)}</t>
+  </si>
+  <si>
+    <t>&lt;jt:agg items="${employees}" aggs="Sum(salary)" valuesVar="values" groupBy="isAManager();title;catchPhrase" cube="${[0, 1, 2]}"&gt;&lt;jt:forEach items="${values}" var="value" orderBy="getPropertyValue(0);getPropertyValue(1);getPropertyValue(2)"&gt;${value.isGrouping(0) ? 'All Values' : value.getPropertyValue(0)}</t>
+  </si>
+  <si>
+    <t>&lt;jt:agg items="${employees}" aggs="Sum(salary)" valuesVar="values" groupBy="isAManager();title;catchPhrase" rollups="${[[1], [2]]}"&gt;&lt;jt:forEach items="${values}" var="value" orderBy="getPropertyValue(0);getPropertyValue(1);getPropertyValue(2)"&gt;${value.isGrouping(0) ? 'All Values' : value.getPropertyValue(0)}</t>
+  </si>
+  <si>
+    <t>&lt;jt:agg items="${employees}" aggs="Sum(salary)" valuesVar="values" groupBy="isAManager();title" rollup="${[0, 1]}"&gt;&lt;jt:forEach items="${values}" var="value" orderBy="getPropertyValue(0);getPropertyValue(1)"&gt;${value.isGrouping(0) ? 'All Values' : value.getPropertyValue(0)}</t>
+  </si>
+  <si>
+    <t>&lt;jt:agg items="${employees}" aggs="Sum(salary)" valuesVar="values" groupBy="isAManager()" useMsd="true"&gt;&lt;jt:forEach items="${values}" var="value"&gt;${value.getPropertyValue(0)}</t>
   </si>
 </sst>
 </file>
@@ -614,7 +614,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>12</v>
@@ -622,7 +622,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>13</v>
@@ -648,7 +648,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>11</v>
@@ -659,10 +659,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>13</v>
@@ -688,13 +688,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>12</v>
@@ -705,10 +705,10 @@
         <v>20</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>13</v>
@@ -734,13 +734,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>12</v>
@@ -748,13 +748,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>13</v>
@@ -780,13 +780,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>12</v>
@@ -794,13 +794,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Enhancements for Tickets 15 and 20.  Upgrade to jAgg 0.8.0 to provide nested properties.  Full Java-like escape characters in attribute values.  New past end action to replace expressions, with a new attribute (and metadata support) to provide a replacement value.  Bug fix: Page Setup settings now preserved on cloned sheets.
</commit_message>
<xml_diff>
--- a/jett-core/templates/AggTagTemplate.xlsx
+++ b/jett-core/templates/AggTagTemplate.xlsx
@@ -68,12 +68,6 @@
     <t>${nevada.name} Counties</t>
   </si>
   <si>
-    <t>&lt;jt:agg items="${california.counties}" aggs="Count(*);Sum(population);StdDev(area)" aggsVar="aggs" valuesVar="values" groupBy="nameFirstLetter"&gt;&lt;jt:forEach items="${values}" var="value"&gt;${value.object.nameFirstLetter}</t>
-  </si>
-  <si>
-    <t>&lt;jt:agg items="${nevada.counties}" aggs="Count(*);Sum(population);StdDev(area)" aggsVar="aggs" valuesVar="values" groupBy="nameFirstLetter"&gt;&lt;jt:forEach items="${values}" var="value"&gt;${value.object.nameFirstLetter}</t>
-  </si>
-  <si>
     <t>${value.getAggregateValue(aggs[2])}&lt;/jt:forEach&gt;&lt;/jt:agg&gt;</t>
   </si>
   <si>
@@ -111,6 +105,12 @@
   </si>
   <si>
     <t>&lt;jt:agg items="${employees}" aggs="Sum(salary)" valuesVar="values" groupBy="isAManager()" useMsd="true"&gt;&lt;jt:forEach items="${values}" var="value"&gt;${value.getPropertyValue(0)}</t>
+  </si>
+  <si>
+    <t>&lt;jt:agg items="${california.counties}" aggs="Count(*);Sum(population);StdDev(area)" aggsVar="aggs" valuesVar="values" groupBy="name.substring(0,1)"&gt;&lt;jt:forEach items="${values}" var="value"&gt;${value.object.nameFirstLetter}</t>
+  </si>
+  <si>
+    <t>&lt;jt:agg items="${nevada.counties}" aggs="Count(*);Sum(population);StdDev(area)" aggsVar="aggs" valuesVar="values" groupBy="name.substring(0,1)"&gt;&lt;jt:forEach items="${values}" var="value"&gt;${value.object.nameFirstLetter}</t>
   </si>
 </sst>
 </file>
@@ -542,7 +542,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -551,7 +551,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -578,7 +578,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>0</v>
@@ -587,7 +587,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -604,7 +604,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -614,18 +616,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -638,7 +640,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -648,24 +652,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -677,7 +681,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -688,30 +694,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>16</v>
-      </c>
       <c r="D1" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="D2" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -734,30 +740,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>16</v>
-      </c>
       <c r="D1" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="D2" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -769,7 +775,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -780,30 +788,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>16</v>
-      </c>
       <c r="D1" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="D2" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>